<commit_message>
K Revert rename Table Description resource column
</commit_message>
<xml_diff>
--- a/R-kds2db/kds2db/inst/extdata/Table_Description.xlsx
+++ b/R-kds2db/kds2db/inst/extdata/Table_Description.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="1882">
   <si>
-    <t xml:space="preserve">table</t>
+    <t xml:space="preserve">resource</t>
   </si>
   <si>
     <t xml:space="preserve">column_name</t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">count</t>
   </si>
   <si>
-    <t xml:space="preserve">encounter</t>
+    <t xml:space="preserve">Encounter</t>
   </si>
   <si>
     <t xml:space="preserve">enc_id</t>
@@ -467,7 +467,7 @@
     <t xml:space="preserve">serviceProvider/display</t>
   </si>
   <si>
-    <t xml:space="preserve">patient</t>
+    <t xml:space="preserve">Patient</t>
   </si>
   <si>
     <t xml:space="preserve">pat_id</t>
@@ -536,7 +536,7 @@
     <t xml:space="preserve">address/postalCode</t>
   </si>
   <si>
-    <t xml:space="preserve">condition</t>
+    <t xml:space="preserve">Condition</t>
   </si>
   <si>
     <t xml:space="preserve">con_id</t>
@@ -1184,7 +1184,7 @@
     <t xml:space="preserve">note/text</t>
   </si>
   <si>
-    <t xml:space="preserve">medication</t>
+    <t xml:space="preserve">Medication</t>
   </si>
   <si>
     <t xml:space="preserve">med_id</t>
@@ -1481,7 +1481,7 @@
     <t xml:space="preserve">boolean</t>
   </si>
   <si>
-    <t xml:space="preserve">medicationrequest</t>
+    <t xml:space="preserve">MedicationRequest</t>
   </si>
   <si>
     <t xml:space="preserve">medreq_id</t>
@@ -2732,7 +2732,7 @@
     <t xml:space="preserve">substitution/reason/text</t>
   </si>
   <si>
-    <t xml:space="preserve">medicationadministration</t>
+    <t xml:space="preserve">MedicationAdministration</t>
   </si>
   <si>
     <t xml:space="preserve">medadm_id</t>
@@ -3194,7 +3194,7 @@
     <t xml:space="preserve">dosage/rateQuantity/code</t>
   </si>
   <si>
-    <t xml:space="preserve">medicationstatement</t>
+    <t xml:space="preserve">MedicationStatement</t>
   </si>
   <si>
     <t xml:space="preserve">medstat_id</t>
@@ -4202,7 +4202,7 @@
     <t xml:space="preserve">dosage/maxDosePerLifetime/code</t>
   </si>
   <si>
-    <t xml:space="preserve">observation</t>
+    <t xml:space="preserve">Observation</t>
   </si>
   <si>
     <t xml:space="preserve">obs_id</t>
@@ -4850,7 +4850,7 @@
     <t xml:space="preserve">hasMember/display</t>
   </si>
   <si>
-    <t xml:space="preserve">diagnosticreport</t>
+    <t xml:space="preserve">DiagnosticReport</t>
   </si>
   <si>
     <t xml:space="preserve">diagrep_id</t>
@@ -5006,7 +5006,7 @@
     <t xml:space="preserve">conclusionCode/text</t>
   </si>
   <si>
-    <t xml:space="preserve">servicerequest</t>
+    <t xml:space="preserve">ServiceRequest</t>
   </si>
   <si>
     <t xml:space="preserve">servreq_id</t>
@@ -5198,7 +5198,7 @@
     <t xml:space="preserve">locationCode/text</t>
   </si>
   <si>
-    <t xml:space="preserve">procedure</t>
+    <t xml:space="preserve">Procedure</t>
   </si>
   <si>
     <t xml:space="preserve">proc_id</t>
@@ -5414,7 +5414,7 @@
     <t xml:space="preserve">proc_note_text</t>
   </si>
   <si>
-    <t xml:space="preserve">consent</t>
+    <t xml:space="preserve">Consent</t>
   </si>
   <si>
     <t xml:space="preserve">cons_id</t>
@@ -5585,7 +5585,7 @@
     <t xml:space="preserve">provision/dataPeriod/end</t>
   </si>
   <si>
-    <t xml:space="preserve">location</t>
+    <t xml:space="preserve">Location</t>
   </si>
   <si>
     <t xml:space="preserve">loc_id</t>

</xml_diff>

<commit_message>
Fix Table Description and SQL Script
</commit_message>
<xml_diff>
--- a/R-kds2db/kds2db/inst/extdata/Table_Description.xlsx
+++ b/R-kds2db/kds2db/inst/extdata/Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="1882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="1881">
   <si>
     <t xml:space="preserve">resource</t>
   </si>
@@ -5645,10 +5645,7 @@
     <t xml:space="preserve">pids_per_ward</t>
   </si>
   <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date+time</t>
+    <t xml:space="preserve">date_time</t>
   </si>
   <si>
     <t xml:space="preserve">ward_name</t>
@@ -23826,23 +23823,23 @@
         <v>1877</v>
       </c>
       <c r="D1163" t="s">
-        <v>1878</v>
+        <v>31</v>
       </c>
       <c r="E1163" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F1163"/>
     </row>
     <row r="1164">
       <c r="A1164"/>
       <c r="B1164" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>1878</v>
+      </c>
+      <c r="D1164" t="s">
         <v>1879</v>
-      </c>
-      <c r="C1164" t="s">
-        <v>1879</v>
-      </c>
-      <c r="D1164" t="s">
-        <v>1880</v>
       </c>
       <c r="E1164" t="n">
         <v>30</v>
@@ -23852,13 +23849,13 @@
     <row r="1165">
       <c r="A1165"/>
       <c r="B1165" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="C1165" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="D1165" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="E1165" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
K Set Condition recordedDate from date to datetime
</commit_message>
<xml_diff>
--- a/R-kds2db/kds2db/inst/extdata/Table_Description.xlsx
+++ b/R-kds2db/kds2db/inst/extdata/Table_Description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-kds2db\kds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE3CAF2-4748-4BF3-B5B6-9B5145825710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE913635-A4CC-4F97-8CA9-A6F9B83AB666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6004,12 +6004,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7974,7 +7975,7 @@
         <v>292</v>
       </c>
       <c r="E154" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="F154">
         <v>30</v>

</xml_diff>